<commit_message>
Import Mapping with sample data
</commit_message>
<xml_diff>
--- a/DHK.Blazor.Server/wwwroot/templates/CourseTemplate.xlsx
+++ b/DHK.Blazor.Server/wwwroot/templates/CourseTemplate.xlsx
@@ -23,6 +23,9 @@
     <t>Program</t>
   </si>
   <si>
+    <t>Unit</t>
+  </si>
+  <si>
     <t>YearLevel</t>
   </si>
   <si>
@@ -33,6 +36,9 @@
   </si>
   <si>
     <t>BSCS</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
   <si>
     <t>FIRST</t>
@@ -380,6 +386,7 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1">
@@ -395,19 +402,25 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>